<commit_message>
fix(49644) Altera modelo xlsx demonstrativo financeiro
Remove caixa de comentário
</commit_message>
<xml_diff>
--- a/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro_novo_v4.xlsx
+++ b/sme_ptrf_apps/static/cargas/modelo_demonstrativo_financeiro_novo_v4.xlsx
@@ -203,33 +203,6 @@
 Saque
 Estorno
 Outros (aberto para digitação)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="A69" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Ou "Documento parcial gerado pelo SIG-Escola, pelo usuário XXXX, em DD/MM/AAAA"</t>
         </r>
       </text>
     </comment>
@@ -2256,9 +2229,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>56160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2272,7 +2245,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="152280"/>
-          <a:ext cx="636840" cy="536400"/>
+          <a:ext cx="636480" cy="536040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2294,11 +2267,11 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>60480</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>531360</xdr:colOff>
+      <xdr:colOff>531000</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
@@ -2313,8 +2286,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="389160" y="178560"/>
-          <a:ext cx="470880" cy="546120"/>
+          <a:off x="4911120" y="178920"/>
+          <a:ext cx="470520" cy="545760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3465,12 +3438,12 @@
   <dimension ref="A2:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
+      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="54.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="1" width="12.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="9.13"/>
@@ -4602,7 +4575,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>